<commit_message>
Add links to MA 115 page.
</commit_message>
<xml_diff>
--- a/teaching/MA-115-FA19/lesson-plans/4/lastname-Lab1.xlsx
+++ b/teaching/MA-115-FA19/lesson-plans/4/lastname-Lab1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\zorak2\users$\ddarmon\Desktop\teaching-files\session4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daviddarmon/Dropbox (Personal)/Reference/T/teaching/201920/2019fa/ma115/lesson-plans/4/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233D6485-BDEB-1541-892A-0ACA388780A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quadratic" sheetId="1" r:id="rId1"/>
@@ -58,8 +59,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,13 +76,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -93,14 +106,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -378,38 +394,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -420,38 +436,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -462,38 +478,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.85546875" customWidth="1"/>
+    <col min="1" max="1" width="56.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>

</xml_diff>